<commit_message>
care bear not working
</commit_message>
<xml_diff>
--- a/PS3/testSets.xlsx
+++ b/PS3/testSets.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="390" windowWidth="12195" windowHeight="7395" activeTab="2"/>
+    <workbookView xWindow="600" yWindow="390" windowWidth="12195" windowHeight="7395" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="sample_scenario1" sheetId="1" r:id="rId1"/>
     <sheet name="sample_scenario2" sheetId="4" r:id="rId2"/>
     <sheet name="sample_scenario3" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="25">
   <si>
     <t>one</t>
   </si>
@@ -76,6 +77,21 @@
   </si>
   <si>
     <t>twenty</t>
+  </si>
+  <si>
+    <t>Set1</t>
+  </si>
+  <si>
+    <t>Set2</t>
+  </si>
+  <si>
+    <t>Justin</t>
+  </si>
+  <si>
+    <t>Dictator</t>
+  </si>
+  <si>
+    <t>Set3</t>
   </si>
 </sst>
 </file>
@@ -615,6 +631,650 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Set1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$B$1:$B$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set1 Justin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$C$1:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set1 Dictator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="148251776"/>
+        <c:axId val="148373888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="148251776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="148373888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="148373888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="148251776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="104"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="4"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Set2</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$B$9:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set2 Justin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$11:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$C$9:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set2 Dictator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$C$11:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="163377920"/>
+        <c:axId val="163379456"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="163377920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="163379456"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="163379456"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="163377920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="105"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="5"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Set3</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$B$17:$B$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set3 Justin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$19:$B$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$C$17:$C$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set3 Dictator</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$C$19:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-20</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="180844416"/>
+        <c:axId val="180845952"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="180844416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180845952"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="180845952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="180844416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>90488</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Chart 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1382,7 +2042,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1614,4 +2274,209 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>-20</v>
+      </c>
+      <c r="C3">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>-20</v>
+      </c>
+      <c r="C4">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>-20</v>
+      </c>
+      <c r="C5">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>-20</v>
+      </c>
+      <c r="C6">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>-20</v>
+      </c>
+      <c r="C7">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>-20</v>
+      </c>
+      <c r="C11">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>-20</v>
+      </c>
+      <c r="C12">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>-20</v>
+      </c>
+      <c r="C13">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>-20</v>
+      </c>
+      <c r="C14">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>-20</v>
+      </c>
+      <c r="C15">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>-20</v>
+      </c>
+      <c r="C19">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>-20</v>
+      </c>
+      <c r="C20">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>-20</v>
+      </c>
+      <c r="C21">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>-20</v>
+      </c>
+      <c r="C22">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>5</v>
+      </c>
+      <c r="B23">
+        <v>-20</v>
+      </c>
+      <c r="C23">
+        <v>-20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>